<commit_message>
added cudaFree before executing gpu_search
</commit_message>
<xml_diff>
--- a/statistics/GPU.xlsx
+++ b/statistics/GPU.xlsx
@@ -33,11 +33,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,19 +287,19 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>4.0</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>8.0</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>16.0</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>32.0</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>64.0</v>
       </c>
     </row>
@@ -307,340 +307,340 @@
       <c r="A2" s="1">
         <v>5.0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.03</v>
       </c>
       <c r="C2" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="D2" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="D2" s="1">
         <v>0.03</v>
       </c>
       <c r="E2" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="F2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F2" s="1">
         <v>0.04</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>10.0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.07</v>
       </c>
       <c r="C3" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.05</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.05</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F3" s="2">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>20.0</v>
       </c>
       <c r="B4" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="C4" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.11</v>
       </c>
       <c r="D4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="2">
         <v>0.11</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="1">
         <v>0.12</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.12</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>40.0</v>
       </c>
       <c r="B5" s="2">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="C5" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.22</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.22</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.22</v>
+        <v>0.28</v>
       </c>
       <c r="F5" s="2">
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>80.0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.48</v>
       </c>
       <c r="C6" s="2">
-        <v>0.52</v>
+        <v>0.43</v>
       </c>
       <c r="D6" s="2">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="E6" s="2">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="F6" s="2">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>4.0</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>8.0</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>16.0</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>32.0</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>64.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>5.0</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.01</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.01</v>
       </c>
       <c r="D10" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E10" s="2">
         <v>0.01</v>
       </c>
+      <c r="E10" s="1">
+        <v>0.01</v>
+      </c>
       <c r="F10" s="2">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>10.0</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="B11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E11" s="1">
         <v>0.03</v>
       </c>
       <c r="F11" s="2">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>20.0</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="E12" s="2">
         <v>0.05</v>
       </c>
-      <c r="C12" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>0.07</v>
       </c>
-      <c r="F12" s="2">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>40.0</v>
       </c>
-      <c r="B13" s="1">
-        <v>0.12</v>
+      <c r="B13" s="2">
+        <v>0.11</v>
       </c>
       <c r="C13" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="E13" s="2">
         <v>0.24</v>
       </c>
-      <c r="D13" s="2">
+      <c r="F13" s="2">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="B14" s="1">
         <v>0.22</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="C14" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="E14" s="2">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.25</v>
-      </c>
       <c r="F14" s="2">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>4.0</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>8.0</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>16.0</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>32.0</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>64.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>5.0</v>
       </c>
       <c r="B17" s="2">
-        <v>0.07</v>
+        <v>0.03</v>
       </c>
       <c r="C17" s="2">
-        <v>0.07</v>
+        <v>0.01</v>
       </c>
       <c r="D17" s="2">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="E17" s="2">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F17" s="2">
-        <v>0.11</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>10.0</v>
       </c>
       <c r="B18" s="2">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="C18" s="2">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="D18" s="2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="E18" s="2">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="F18" s="2">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>20.0</v>
       </c>
       <c r="B19" s="2">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="C19" s="2">
-        <v>0.16</v>
+        <v>0.05</v>
       </c>
       <c r="D19" s="2">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="E19" s="2">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="F19" s="2">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>40.0</v>
       </c>
       <c r="B20" s="2">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="C20" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.2</v>
+        <v>0.12</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.14</v>
       </c>
       <c r="F20" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="B21" s="2">
         <v>0.28</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.36</v>
-      </c>
       <c r="C21" s="2">
-        <v>0.34</v>
+        <v>0.21</v>
       </c>
       <c r="D21" s="2">
-        <v>0.31</v>
+        <v>0.27</v>
       </c>
       <c r="E21" s="2">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="F21" s="2">
-        <v>0.29</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -659,140 +659,140 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.04</v>
       </c>
       <c r="D2" s="2">
-        <v>0.14</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.1</v>
       </c>
       <c r="C3" s="2">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="D3" s="2">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>4.0</v>
       </c>
       <c r="B4" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="C4" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.04</v>
       </c>
       <c r="D4" s="2">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>8.0</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.04</v>
       </c>
       <c r="D5" s="2">
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>16.0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.56</v>
       </c>
       <c r="C6" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.37</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>128.0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.58</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>256.0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9.12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="D10" s="2">
         <v>0.05</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>32.0</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1.21</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>64.0</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2.37</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>128.0</v>
-      </c>
-      <c r="B9" s="2">
-        <v>4.61</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
-        <v>256.0</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9.06</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>